<commit_message>
fix temporal coverage error and clean up script
</commit_message>
<xml_diff>
--- a/nes-lter-growth-grazing-chl-info.xlsx
+++ b/nes-lter-growth-grazing-chl-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-growth-grazing-chl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB43B2-C408-4106-AED1-02CACAA3E01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D2FB60-61FA-48F3-AA7E-188072648D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
@@ -541,7 +541,7 @@
     <t>Not nutrient-limited, thus no value.</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
+    <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
adjust all missing value codes to NaN
</commit_message>
<xml_diff>
--- a/nes-lter-growth-grazing-chl-info.xlsx
+++ b/nes-lter-growth-grazing-chl-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-growth-grazing-chl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D2FB60-61FA-48F3-AA7E-188072648D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD24790-9D0B-4A88-B5E4-4D845004BA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="170">
   <si>
     <t>givenName</t>
   </si>
@@ -535,13 +535,10 @@
     <t>Not available</t>
   </si>
   <si>
-    <t>n/n</t>
-  </si>
-  <si>
     <t>Not nutrient-limited, thus no value.</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
+    <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
 </sst>
 </file>
@@ -611,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -651,9 +648,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -971,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F47B1D1-85BF-498C-B80C-7A27FBFE6C7D}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1059,7 @@
         <v>151</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1079,7 +1073,7 @@
         <v>151</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1093,7 +1087,7 @@
         <v>151</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1307,7 +1301,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1428,11 +1422,11 @@
       <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1448,11 +1442,11 @@
       <c r="D30" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
methods and keywords edits
</commit_message>
<xml_diff>
--- a/nes-lter-growth-grazing-chl-info.xlsx
+++ b/nes-lter-growth-grazing-chl-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-growth-grazing-chl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD24790-9D0B-4A88-B5E4-4D845004BA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2192D9CB-61A0-4B01-B3C8-EFF9583CC274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="-19488" yWindow="-1080" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="168">
   <si>
     <t>givenName</t>
   </si>
@@ -242,12 +242,6 @@
   </si>
   <si>
     <t>Marine</t>
-  </si>
-  <si>
-    <t>Phytoplankton growth</t>
-  </si>
-  <si>
-    <t>Zooplankton growth</t>
   </si>
   <si>
     <t>categorical</t>
@@ -965,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F47B1D1-85BF-498C-B80C-7A27FBFE6C7D}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+    <sheetView topLeftCell="C15" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -1009,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
@@ -1020,7 +1014,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>34</v>
@@ -1028,10 +1022,10 @@
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
@@ -1050,44 +1044,44 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1095,7 +1089,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -1109,7 +1103,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -1123,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>35</v>
@@ -1134,139 +1128,139 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>35</v>
@@ -1275,18 +1269,18 @@
         <v>36</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>35</v>
@@ -1295,32 +1289,32 @@
         <v>36</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>35</v>
@@ -1334,39 +1328,39 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1374,24 +1368,24 @@
         <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>62</v>
@@ -1400,13 +1394,13 @@
         <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1414,50 +1408,50 @@
         <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1488,238 +1482,238 @@
         <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="11">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="11">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="11">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="10">
         <v>0.01</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="10">
         <v>0.03</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="10">
         <v>0.05</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="10">
         <v>0.1</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="10">
         <v>0.15</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="10">
         <v>0.3</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="10">
         <v>0.65</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="6">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" s="6">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="6">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="6">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1767,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9149FEFC-E904-AF4E-BB9C-B9D79FB8550A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1867,21 +1861,11 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
+      <c r="A12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1924,19 +1908,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2073,7 +2057,7 @@
         <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -2110,22 +2094,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
         <v>80</v>
-      </c>
-      <c r="F6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>82</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
incorporate removal of special size fraction & text edits
</commit_message>
<xml_diff>
--- a/nes-lter-growth-grazing-chl-info.xlsx
+++ b/nes-lter-growth-grazing-chl-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-growth-grazing-chl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2192D9CB-61A0-4B01-B3C8-EFF9583CC274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD182AC-27E6-47B7-B599-8F29831EC503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19488" yWindow="-1080" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="166">
   <si>
     <t>givenName</t>
   </si>
@@ -358,9 +358,6 @@
     <t>Size fraction of the computed rate</t>
   </si>
   <si>
-    <t>&gt;0&amp;&lt;10sf</t>
-  </si>
-  <si>
     <t>&gt;10&amp;&lt;200</t>
   </si>
   <si>
@@ -461,9 +458,6 @@
   </si>
   <si>
     <t>Standard deviation of the temperature during the incubation</t>
-  </si>
-  <si>
-    <t>size fraction of the computed rate is 0.7 to 10 microns and sample is from an experiment</t>
   </si>
   <si>
     <t>size fraction of the computed rate is greater than 0.7 microns (no prefilter used)</t>
@@ -959,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F47B1D1-85BF-498C-B80C-7A27FBFE6C7D}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="C15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -1003,7 +997,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
@@ -1014,7 +1008,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>34</v>
@@ -1025,7 +1019,7 @@
         <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
@@ -1047,13 +1041,13 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1064,10 +1058,10 @@
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1078,10 +1072,10 @@
         <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1089,7 +1083,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -1103,7 +1097,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -1117,7 +1111,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>35</v>
@@ -1131,7 +1125,7 @@
         <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>35</v>
@@ -1145,7 +1139,7 @@
         <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>71</v>
@@ -1156,7 +1150,7 @@
         <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>35</v>
@@ -1170,7 +1164,7 @@
         <v>93</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>35</v>
@@ -1184,7 +1178,7 @@
         <v>92</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>71</v>
@@ -1206,13 +1200,13 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1220,19 +1214,19 @@
         <v>89</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1240,19 +1234,19 @@
         <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1260,7 +1254,7 @@
         <v>87</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>35</v>
@@ -1269,10 +1263,10 @@
         <v>36</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1280,7 +1274,7 @@
         <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>35</v>
@@ -1289,10 +1283,10 @@
         <v>36</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1306,7 +1300,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1314,7 +1308,7 @@
         <v>84</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>35</v>
@@ -1328,7 +1322,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>35</v>
@@ -1337,18 +1331,18 @@
         <v>73</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>35</v>
@@ -1357,10 +1351,10 @@
         <v>73</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1368,7 +1362,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>35</v>
@@ -1377,15 +1371,15 @@
         <v>73</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>62</v>
@@ -1397,10 +1391,10 @@
         <v>73</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1408,7 +1402,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>35</v>
@@ -1417,18 +1411,18 @@
         <v>73</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>35</v>
@@ -1437,10 +1431,10 @@
         <v>73</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1448,7 +1442,7 @@
         <v>83</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>71</v>
@@ -1462,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6E3299-91E1-468F-8923-DC80CDD536C5}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1504,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1526,7 +1520,7 @@
         <v>0.01</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1537,7 +1531,7 @@
         <v>0.03</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,7 +1542,7 @@
         <v>0.05</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,7 +1553,7 @@
         <v>0.1</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,7 +1564,7 @@
         <v>0.15</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1581,7 +1575,7 @@
         <v>0.3</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1592,7 +1586,7 @@
         <v>0.65</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1603,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,7 +1608,7 @@
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1622,10 +1616,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1633,10 +1627,10 @@
         <v>91</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1644,21 +1638,21 @@
         <v>91</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>109</v>
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1666,10 +1660,10 @@
         <v>83</v>
       </c>
       <c r="B18" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1677,10 +1671,10 @@
         <v>83</v>
       </c>
       <c r="B19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1688,10 +1682,10 @@
         <v>83</v>
       </c>
       <c r="B20" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1699,33 +1693,31 @@
         <v>83</v>
       </c>
       <c r="B21" s="6">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="6">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
@@ -1734,7 +1726,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="5"/>
@@ -1742,15 +1734,6 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1763,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9149FEFC-E904-AF4E-BB9C-B9D79FB8550A}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD13"/>
+    <sheetView topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,10 +1897,10 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
         <v>119</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
       </c>
       <c r="E2" t="s">
         <v>74</v>
@@ -2057,7 +2040,7 @@
         <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>

</xml_diff>